<commit_message>
Organize test case by feature
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cell-text" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="194">
   <si>
     <t>autofilter</t>
   </si>
@@ -520,9 +520,6 @@
     <t>inner</t>
   </si>
   <si>
-    <t>dot</t>
-  </si>
-  <si>
     <t>borders inside</t>
   </si>
   <si>
@@ -548,9 +545,6 @@
   </si>
   <si>
     <t>dashed</t>
-  </si>
-  <si>
-    <t>big dot</t>
   </si>
   <si>
     <t>dot-dashed</t>
@@ -619,6 +613,12 @@
   </si>
   <si>
     <t>double accounting</t>
+  </si>
+  <si>
+    <t>hair</t>
+  </si>
+  <si>
+    <t>dotted</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1038,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -1384,28 +1384,6 @@
     <border>
       <left/>
       <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="mediumDashDotDot">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="dashDotDot">
         <color auto="1"/>
       </top>
@@ -1566,7 +1544,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1749,10 +1727,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
@@ -1760,9 +1738,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1783,13 +1766,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1948,7 +1924,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1968,10 +1944,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15789749537121869"/>
+          <c:x val="0.1578974953712188"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.58796850393700628"/>
-          <c:h val="0.76578566465956688"/>
+          <c:w val="0.58796850393700606"/>
+          <c:h val="0.76578566465956732"/>
         </c:manualLayout>
       </c:layout>
       <c:area3DChart>
@@ -2198,25 +2174,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="90183552"/>
-        <c:axId val="90185088"/>
-        <c:axId val="77358848"/>
+        <c:axId val="76891264"/>
+        <c:axId val="76892800"/>
+        <c:axId val="76837760"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="90183552"/>
+        <c:axId val="76891264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90185088"/>
+        <c:crossAx val="76892800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90185088"/>
+        <c:axId val="76892800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2224,18 +2200,18 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90183552"/>
+        <c:crossAx val="76891264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="77358848"/>
+        <c:axId val="76837760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90185088"/>
+        <c:crossAx val="76892800"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2249,7 +2225,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2500,22 +2476,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="90277376"/>
-        <c:axId val="90278912"/>
+        <c:axId val="76980992"/>
+        <c:axId val="76982528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90277376"/>
+        <c:axId val="76980992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90278912"/>
+        <c:crossAx val="76982528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90278912"/>
+        <c:axId val="76982528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2523,7 +2499,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90277376"/>
+        <c:crossAx val="76980992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2535,7 +2511,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2797,7 +2773,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3062,7 +3038,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3394,22 +3370,22 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="90430848"/>
-        <c:axId val="90444928"/>
+        <c:axId val="78162560"/>
+        <c:axId val="78176640"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="90430848"/>
+        <c:axId val="78162560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90444928"/>
+        <c:crossAx val="78176640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90444928"/>
+        <c:axId val="78176640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3417,7 +3393,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90430848"/>
+        <c:crossAx val="78162560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3429,7 +3405,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3674,25 +3650,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="90457984"/>
-        <c:axId val="90459520"/>
+        <c:axId val="78304384"/>
+        <c:axId val="78305920"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="90457984"/>
+        <c:axId val="78304384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90459520"/>
+        <c:crossAx val="78305920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90459520"/>
+        <c:axId val="78305920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3700,7 +3676,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90457984"/>
+        <c:crossAx val="78304384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3712,7 +3688,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3811,8 +3787,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.70019920318725093"/>
           <c:y val="0.18529458333168791"/>
-          <c:w val="0.25885988970479873"/>
-          <c:h val="0.56509104330708804"/>
+          <c:w val="0.2588598897047989"/>
+          <c:h val="0.56509104330708826"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -3831,7 +3807,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4068,24 +4044,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="75344512"/>
-        <c:axId val="75358592"/>
+        <c:axId val="58771328"/>
+        <c:axId val="58772864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75344512"/>
+        <c:axId val="58771328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75358592"/>
+        <c:crossAx val="58772864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75358592"/>
+        <c:axId val="58772864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4093,7 +4069,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75344512"/>
+        <c:crossAx val="58771328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4105,7 +4081,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4346,25 +4322,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="76813824"/>
-        <c:axId val="76815360"/>
+        <c:axId val="58782464"/>
+        <c:axId val="58784000"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="76813824"/>
+        <c:axId val="58782464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76815360"/>
+        <c:crossAx val="58784000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76815360"/>
+        <c:axId val="58784000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4372,7 +4348,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76813824"/>
+        <c:crossAx val="58782464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4384,7 +4360,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4630,24 +4606,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76857344"/>
-        <c:axId val="76858880"/>
+        <c:axId val="60730368"/>
+        <c:axId val="60748544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76857344"/>
+        <c:axId val="60730368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76858880"/>
+        <c:crossAx val="60748544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76858880"/>
+        <c:axId val="60748544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4655,7 +4631,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76857344"/>
+        <c:crossAx val="60730368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4667,7 +4643,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4906,25 +4882,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="77281920"/>
-        <c:axId val="77291904"/>
-        <c:axId val="76862336"/>
+        <c:axId val="75696000"/>
+        <c:axId val="75697536"/>
+        <c:axId val="60702208"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="77281920"/>
+        <c:axId val="75696000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77291904"/>
+        <c:crossAx val="75697536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77291904"/>
+        <c:axId val="75697536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4932,19 +4908,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77281920"/>
+        <c:crossAx val="75696000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="76862336"/>
+        <c:axId val="60702208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="77291904"/>
+        <c:crossAx val="75697536"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -4955,7 +4931,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5192,24 +5168,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="77318400"/>
-        <c:axId val="77336576"/>
+        <c:axId val="75716096"/>
+        <c:axId val="75717632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77318400"/>
+        <c:axId val="75716096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77336576"/>
+        <c:crossAx val="75717632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77336576"/>
+        <c:axId val="75717632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5217,7 +5193,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77318400"/>
+        <c:crossAx val="75716096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5229,7 +5205,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5251,7 +5227,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.25918955252544651"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.50321397186770522"/>
+          <c:w val="0.50321397186770478"/>
           <c:h val="0.8221582606228276"/>
         </c:manualLayout>
       </c:layout>
@@ -5481,25 +5457,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="77354496"/>
-        <c:axId val="77356032"/>
+        <c:axId val="76808960"/>
+        <c:axId val="76810496"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="77354496"/>
+        <c:axId val="76808960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77356032"/>
+        <c:crossAx val="76810496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77356032"/>
+        <c:axId val="76810496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5507,7 +5483,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77354496"/>
+        <c:crossAx val="76808960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5522,7 +5498,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5758,24 +5734,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="77372800"/>
-        <c:axId val="77390976"/>
+        <c:axId val="76819072"/>
+        <c:axId val="76870016"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="77372800"/>
+        <c:axId val="76819072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77390976"/>
+        <c:crossAx val="76870016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77390976"/>
+        <c:axId val="76870016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5783,7 +5759,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77372800"/>
+        <c:crossAx val="76819072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5795,7 +5771,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6631,7 +6607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -6674,17 +6650,17 @@
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
@@ -6714,7 +6690,7 @@
       <c r="H4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="121" t="s">
+      <c r="I4" s="119" t="s">
         <v>24</v>
       </c>
       <c r="J4" s="17" t="s">
@@ -6725,7 +6701,7 @@
       </c>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:13" ht="64.5">
+    <row r="5" spans="1:13" ht="48.75">
       <c r="A5" s="19" t="s">
         <v>27</v>
       </c>
@@ -6756,17 +6732,17 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="123" t="s">
-        <v>184</v>
-      </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="123"/>
+      <c r="B6" s="124" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
     </row>
     <row r="7" spans="1:13" ht="92.25">
       <c r="A7" s="23" t="s">
@@ -6819,14 +6795,14 @@
       <c r="D10" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="138" t="s">
+      <c r="E10" s="120" t="s">
+        <v>189</v>
+      </c>
+      <c r="F10" s="121" t="s">
+        <v>190</v>
+      </c>
+      <c r="G10" s="122" t="s">
         <v>191</v>
-      </c>
-      <c r="F10" s="139" t="s">
-        <v>192</v>
-      </c>
-      <c r="G10" s="140" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="21">
@@ -6933,7 +6909,7 @@
     </row>
     <row r="26" spans="1:4" ht="60">
       <c r="B26" s="94" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="48.75" customHeight="1">
@@ -7157,13 +7133,13 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
@@ -7184,14 +7160,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
@@ -7201,7 +7178,7 @@
     <col min="12" max="12" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21">
+    <row r="1" spans="1:7" ht="21">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -7215,13 +7192,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="21">
+    <row r="2" spans="1:7" ht="21">
       <c r="A2" s="4"/>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
       <c r="D2" s="59"/>
     </row>
-    <row r="3" spans="1:12" ht="21">
+    <row r="3" spans="1:7" ht="21">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -7238,37 +7215,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:7">
       <c r="B5" s="99" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>171</v>
-      </c>
-      <c r="D5" s="101"/>
-      <c r="E5" s="102" t="s">
-        <v>172</v>
-      </c>
-      <c r="F5" s="103" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1">
-      <c r="B6" s="104" t="s">
-        <v>173</v>
-      </c>
-      <c r="C6" s="105"/>
-      <c r="D6" s="106" t="s">
-        <v>170</v>
-      </c>
-      <c r="E6" s="107"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="109" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="9" spans="1:12">
+        <v>193</v>
+      </c>
+      <c r="D5" s="103" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="B9" s="63" t="s">
         <v>58</v>
       </c>
@@ -7276,19 +7234,13 @@
         <v>59</v>
       </c>
       <c r="E9" s="64" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F9" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="I9" s="69" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1">
+    </row>
+    <row r="10" spans="1:7">
       <c r="B10" s="63" t="s">
         <v>61</v>
       </c>
@@ -7297,78 +7249,35 @@
       </c>
       <c r="E10" s="66"/>
       <c r="F10" s="67"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="71"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="12" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
+    </row>
+    <row r="12" spans="1:7">
       <c r="B12" s="67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C12" s="66"/>
-      <c r="E12" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="72" t="s">
-        <v>59</v>
-      </c>
       <c r="G12" s="59"/>
-      <c r="H12" s="112" t="s">
-        <v>165</v>
-      </c>
-      <c r="I12" s="112" t="s">
-        <v>166</v>
-      </c>
-      <c r="K12" s="113" t="s">
-        <v>165</v>
-      </c>
-      <c r="L12" s="113" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
+    </row>
+    <row r="13" spans="1:7">
       <c r="B13" s="65"/>
       <c r="C13" s="64"/>
-      <c r="E13" s="72" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="112" t="s">
-        <v>175</v>
-      </c>
-      <c r="I13" s="112"/>
-      <c r="K13" s="113" t="s">
-        <v>176</v>
-      </c>
-      <c r="L13" s="113"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickTop="1">
+    </row>
+    <row r="14" spans="1:7">
       <c r="B14" s="59"/>
       <c r="C14" s="59"/>
       <c r="E14" s="59"/>
       <c r="F14" s="59"/>
     </row>
-    <row r="15" spans="1:12">
-      <c r="B15" s="114" t="s">
+    <row r="15" spans="1:7">
+      <c r="B15" s="113" t="s">
         <v>177</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="114"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="115" t="s">
         <v>178</v>
       </c>
-      <c r="E15" s="115" t="s">
-        <v>179</v>
-      </c>
-      <c r="F15" s="116"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="E16" s="117" t="s">
-        <v>180</v>
-      </c>
-      <c r="F16" s="118"/>
+      <c r="C16" s="116"/>
     </row>
     <row r="17" spans="1:8">
       <c r="B17" s="59"/>
@@ -7376,144 +7285,150 @@
       <c r="E17" s="59"/>
       <c r="F17" s="59"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75">
-      <c r="A18" s="33" t="s">
+    <row r="18" spans="1:8">
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75">
+      <c r="A19" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B19" s="64" t="s">
         <v>159</v>
       </c>
-      <c r="C18" s="60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D18" s="65" t="s">
+      <c r="C19" s="60" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="67" t="s">
+      <c r="F19" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="G18" s="95" t="s">
+      <c r="G19" s="95" t="s">
         <v>160</v>
       </c>
-      <c r="H18" s="66" t="s">
+      <c r="H19" s="66" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="B19" s="61"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="62"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="97"/>
-    </row>
     <row r="20" spans="1:8">
-      <c r="B20" s="66"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="67"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="64"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="B22" s="110" t="s">
+      <c r="B20" s="61"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="62"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="97"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" s="66"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="67"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="64"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="B23" s="108" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="108" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="108" t="s">
+        <v>159</v>
+      </c>
+      <c r="F23" s="109" t="s">
         <v>163</v>
       </c>
-      <c r="C22" s="110" t="s">
+      <c r="G23" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="110" t="s">
+      <c r="H23" s="109" t="s">
         <v>159</v>
       </c>
-      <c r="F22" s="111" t="s">
-        <v>164</v>
-      </c>
-      <c r="G22" s="111" t="s">
+    </row>
+    <row r="24" spans="1:8">
+      <c r="B24" s="108" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="111" t="s">
+      <c r="D24" s="108" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="B23" s="110" t="s">
+      <c r="F24" s="109" t="s">
         <v>163</v>
       </c>
-      <c r="C23" s="110" t="s">
+      <c r="G24" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="110" t="s">
+      <c r="H24" s="109" t="s">
         <v>159</v>
       </c>
-      <c r="F23" s="111" t="s">
-        <v>164</v>
-      </c>
-      <c r="G23" s="111" t="s">
+    </row>
+    <row r="25" spans="1:8">
+      <c r="B25" s="108" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="H23" s="111" t="s">
+      <c r="D25" s="108" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="B24" s="110" t="s">
+      <c r="F25" s="109" t="s">
         <v>163</v>
       </c>
-      <c r="C24" s="110" t="s">
+      <c r="G25" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="110" t="s">
+      <c r="H25" s="109" t="s">
         <v>159</v>
       </c>
-      <c r="F24" s="111" t="s">
-        <v>164</v>
-      </c>
-      <c r="G24" s="111" t="s">
-        <v>59</v>
-      </c>
-      <c r="H24" s="111" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="21">
-      <c r="A27" s="4" t="s">
+    </row>
+    <row r="28" spans="1:8" ht="21">
+      <c r="A28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="124" t="s">
+      <c r="B28" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="125"/>
-      <c r="E27" s="124" t="s">
+      <c r="C28" s="126"/>
+      <c r="E28" s="125" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="126"/>
-      <c r="G27" s="125"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="B30" s="127" t="s">
+      <c r="F28" s="127"/>
+      <c r="G28" s="126"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" s="128" t="s">
         <v>157</v>
       </c>
-      <c r="C30" s="130" t="s">
+      <c r="C31" s="131" t="s">
         <v>158</v>
       </c>
-      <c r="D30" s="131"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="B31" s="128"/>
-      <c r="C31" s="132"/>
-      <c r="D31" s="133"/>
+      <c r="D31" s="132"/>
     </row>
     <row r="32" spans="1:8">
       <c r="B32" s="129"/>
-      <c r="C32" s="134"/>
-      <c r="D32" s="135"/>
+      <c r="C32" s="133"/>
+      <c r="D32" s="134"/>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="130"/>
+      <c r="C33" s="135"/>
+      <c r="D33" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:D32"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:D33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7524,7 +7439,7 @@
   <dimension ref="A2:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7532,7 +7447,8 @@
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
@@ -7555,29 +7471,29 @@
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
       <c r="D4" s="101" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E4" s="102" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1">
-      <c r="B5" s="119" t="s">
-        <v>173</v>
-      </c>
-      <c r="C5" s="120" t="s">
-        <v>189</v>
-      </c>
-      <c r="D5" s="106" t="s">
-        <v>170</v>
-      </c>
-      <c r="E5" s="107" t="s">
+      <c r="B5" s="117" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="118" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="104" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="108" t="s">
-        <v>190</v>
-      </c>
-      <c r="G5" s="109" t="s">
+      <c r="F5" s="106" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" s="107" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7610,36 +7526,36 @@
       <c r="G11" s="59"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="B12" s="114" t="s">
-        <v>177</v>
+      <c r="B12" s="112" t="s">
+        <v>175</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>178</v>
-      </c>
-      <c r="E12" s="112" t="s">
+        <v>176</v>
+      </c>
+      <c r="E12" s="110" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" s="110" t="s">
         <v>165</v>
       </c>
-      <c r="F12" s="112" t="s">
-        <v>166</v>
-      </c>
-      <c r="H12" s="113" t="s">
+      <c r="H12" s="111" t="s">
+        <v>164</v>
+      </c>
+      <c r="I12" s="111" t="s">
         <v>165</v>
-      </c>
-      <c r="I12" s="113" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="B13" s="63"/>
       <c r="C13" s="63"/>
-      <c r="E13" s="112" t="s">
-        <v>175</v>
-      </c>
-      <c r="F13" s="112"/>
-      <c r="H13" s="113" t="s">
-        <v>176</v>
-      </c>
-      <c r="I13" s="113"/>
+      <c r="E13" s="110" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13" s="110"/>
+      <c r="H13" s="111" t="s">
+        <v>174</v>
+      </c>
+      <c r="I13" s="111"/>
     </row>
     <row r="16" spans="1:9">
       <c r="B16" s="59"/>
@@ -7758,7 +7674,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="85" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
         <v>93</v>
@@ -7778,10 +7694,10 @@
     </row>
     <row r="11" spans="1:8" ht="21">
       <c r="A11" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B11" s="85" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C11">
         <f>SUM(TestRange1)</f>
@@ -7789,7 +7705,7 @@
       </c>
       <c r="D11" s="59"/>
       <c r="F11" s="85" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G11">
         <f>SUM(RangeMerged,F14:H14)</f>
@@ -7806,11 +7722,11 @@
       <c r="D12" s="65">
         <v>3</v>
       </c>
-      <c r="F12" s="130">
+      <c r="F12" s="131">
         <v>1</v>
       </c>
-      <c r="G12" s="136"/>
-      <c r="H12" s="131"/>
+      <c r="G12" s="137"/>
+      <c r="H12" s="132"/>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" s="66">
@@ -7822,9 +7738,9 @@
       <c r="D13" s="67">
         <v>6</v>
       </c>
-      <c r="F13" s="134"/>
-      <c r="G13" s="137"/>
-      <c r="H13" s="135"/>
+      <c r="F13" s="135"/>
+      <c r="G13" s="138"/>
+      <c r="H13" s="136"/>
     </row>
     <row r="14" spans="1:8">
       <c r="F14">
@@ -7885,7 +7801,7 @@
     <row r="2" spans="1:3" ht="31.5">
       <c r="A2" s="86"/>
       <c r="B2" s="87" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C2">
         <f>SUM([1]Sheet1!$A$3:$C$4)</f>
@@ -7898,10 +7814,10 @@
     </row>
     <row r="4" spans="1:3" ht="61.5">
       <c r="A4" s="86" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" s="87" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C4" t="str">
         <f>row!A1</f>
@@ -7910,7 +7826,7 @@
     </row>
     <row r="5" spans="1:3" ht="45">
       <c r="B5" s="87" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C5">
         <f>SUM('cell-data'!F14:H14)</f>

</xml_diff>

<commit_message>
* add test for "cell-data", "chart-image" * add SpreadsheetAgent to simulate user actions.
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="cell-text" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="193">
   <si>
     <t>autofilter</t>
   </si>
@@ -449,9 +449,6 @@
   </si>
   <si>
     <t>3D bar</t>
-  </si>
-  <si>
-    <t>exploded Doungnet</t>
   </si>
   <si>
     <t>ZSS not support</t>
@@ -1924,7 +1921,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1944,10 +1941,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1578974953712188"/>
+          <c:x val="0.15789749537121886"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.58796850393700606"/>
-          <c:h val="0.76578566465956732"/>
+          <c:w val="0.58796850393700595"/>
+          <c:h val="0.76578566465956754"/>
         </c:manualLayout>
       </c:layout>
       <c:area3DChart>
@@ -2174,25 +2171,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="76891264"/>
-        <c:axId val="76892800"/>
-        <c:axId val="76837760"/>
+        <c:axId val="60948864"/>
+        <c:axId val="60950400"/>
+        <c:axId val="96341504"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="76891264"/>
+        <c:axId val="60948864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76892800"/>
+        <c:crossAx val="60950400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76892800"/>
+        <c:axId val="60950400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2200,23 +2197,24 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76891264"/>
+        <c:crossAx val="60948864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="76837760"/>
+        <c:axId val="96341504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76892800"/>
+        <c:crossAx val="60950400"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2225,7 +2223,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2476,22 +2474,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="76980992"/>
-        <c:axId val="76982528"/>
+        <c:axId val="60960768"/>
+        <c:axId val="60962304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76980992"/>
+        <c:axId val="60960768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76982528"/>
+        <c:crossAx val="60962304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76982528"/>
+        <c:axId val="60962304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2499,19 +2497,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76980992"/>
+        <c:crossAx val="60960768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2768,283 +2767,19 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:doughnutChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'chart-image'!$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Internet Explorer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="25"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'chart-image'!$A$14:$A$20</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>January 2012</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>February 2012</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>March 2012</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>April 2012</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>May 2012</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>June 2012</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>July 2012</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'chart-image'!$B$14:$B$20</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.3427</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.32700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.31680000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.30809999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.28870000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.28949999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.28489999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'chart-image'!$C$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Chrome</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="25"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'chart-image'!$A$14:$A$20</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>January 2012</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>February 2012</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>March 2012</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>April 2012</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>May 2012</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>June 2012</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>July 2012</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'chart-image'!$C$14:$C$20</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.25990000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.27239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.28089999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.28239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.29149999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.29349999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.30059999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'chart-image'!$D$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Firefox</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="25"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'chart-image'!$A$14:$A$20</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>January 2012</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>February 2012</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>March 2012</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>April 2012</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>May 2012</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>June 2012</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>July 2012</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'chart-image'!$D$14:$D$20</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.2268</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2276</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.2273</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.22489999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.22969999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.21010000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="0"/>
-        <c:holeSize val="50"/>
-      </c:doughnutChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3370,22 +3105,22 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="78162560"/>
-        <c:axId val="78176640"/>
+        <c:axId val="75749248"/>
+        <c:axId val="75750784"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="78162560"/>
+        <c:axId val="75749248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78176640"/>
+        <c:crossAx val="75750784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78176640"/>
+        <c:axId val="75750784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3393,7 +3128,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78162560"/>
+        <c:crossAx val="75749248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3405,13 +3140,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3650,25 +3385,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="78304384"/>
-        <c:axId val="78305920"/>
+        <c:axId val="75862400"/>
+        <c:axId val="75863936"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="78304384"/>
+        <c:axId val="75862400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78305920"/>
+        <c:crossAx val="75863936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78305920"/>
+        <c:axId val="75863936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3676,7 +3411,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78304384"/>
+        <c:crossAx val="75862400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3688,7 +3423,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3787,8 +3522,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.70019920318725093"/>
           <c:y val="0.18529458333168791"/>
-          <c:w val="0.2588598897047989"/>
-          <c:h val="0.56509104330708826"/>
+          <c:w val="0.25885988970479895"/>
+          <c:h val="0.56509104330708848"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -3807,7 +3542,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4044,24 +3779,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="58771328"/>
-        <c:axId val="58772864"/>
+        <c:axId val="90990080"/>
+        <c:axId val="91384064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58771328"/>
+        <c:axId val="90990080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58772864"/>
+        <c:crossAx val="91384064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58772864"/>
+        <c:axId val="91384064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4069,7 +3804,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58771328"/>
+        <c:crossAx val="90990080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4081,7 +3816,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4322,25 +4057,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="58782464"/>
-        <c:axId val="58784000"/>
+        <c:axId val="95118080"/>
+        <c:axId val="95151232"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="58782464"/>
+        <c:axId val="95118080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58784000"/>
+        <c:crossAx val="95151232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58784000"/>
+        <c:axId val="95151232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4348,7 +4083,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58782464"/>
+        <c:crossAx val="95118080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4360,7 +4095,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4606,24 +4341,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="60730368"/>
-        <c:axId val="60748544"/>
+        <c:axId val="124593280"/>
+        <c:axId val="124596992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60730368"/>
+        <c:axId val="124593280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60748544"/>
+        <c:crossAx val="124596992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60748544"/>
+        <c:axId val="124596992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4631,7 +4366,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60730368"/>
+        <c:crossAx val="124593280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4643,7 +4378,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4882,25 +4617,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="75696000"/>
-        <c:axId val="75697536"/>
-        <c:axId val="60702208"/>
+        <c:axId val="58766464"/>
+        <c:axId val="58768000"/>
+        <c:axId val="78172608"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="75696000"/>
+        <c:axId val="58766464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75697536"/>
+        <c:crossAx val="58768000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75697536"/>
+        <c:axId val="58768000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4908,19 +4643,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75696000"/>
+        <c:crossAx val="58766464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="60702208"/>
+        <c:axId val="78172608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="75697536"/>
+        <c:crossAx val="58768000"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -4931,7 +4666,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5168,24 +4903,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="75716096"/>
-        <c:axId val="75717632"/>
+        <c:axId val="58782464"/>
+        <c:axId val="58784000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75716096"/>
+        <c:axId val="58782464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75717632"/>
+        <c:crossAx val="58784000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75717632"/>
+        <c:axId val="58784000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5193,7 +4928,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75716096"/>
+        <c:crossAx val="58782464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5205,7 +4940,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5227,7 +4962,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.25918955252544651"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.50321397186770478"/>
+          <c:w val="0.50321397186770456"/>
           <c:h val="0.8221582606228276"/>
         </c:manualLayout>
       </c:layout>
@@ -5457,25 +5192,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="76808960"/>
-        <c:axId val="76810496"/>
+        <c:axId val="60546432"/>
+        <c:axId val="60699776"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="76808960"/>
+        <c:axId val="60546432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76810496"/>
+        <c:crossAx val="60699776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76810496"/>
+        <c:axId val="60699776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5483,7 +5218,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76808960"/>
+        <c:crossAx val="60546432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5498,7 +5233,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5734,24 +5469,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="76819072"/>
-        <c:axId val="76870016"/>
+        <c:axId val="60729216"/>
+        <c:axId val="60730752"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="76819072"/>
+        <c:axId val="60729216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76870016"/>
+        <c:crossAx val="60730752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76870016"/>
+        <c:axId val="60730752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5759,19 +5494,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76819072"/>
+        <c:crossAx val="60729216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6176,36 +5912,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>136</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="20" name="Chart 19"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6733,7 +6439,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="124" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C6" s="124"/>
       <c r="D6" s="124"/>
@@ -6796,13 +6502,13 @@
         <v>40</v>
       </c>
       <c r="E10" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="121" t="s">
         <v>189</v>
       </c>
-      <c r="F10" s="121" t="s">
+      <c r="G10" s="122" t="s">
         <v>190</v>
-      </c>
-      <c r="G10" s="122" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="21">
@@ -6863,14 +6569,14 @@
     </row>
     <row r="20" spans="1:4" ht="21">
       <c r="A20" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D20" s="92"/>
     </row>
     <row r="21" spans="1:4" ht="18.75">
       <c r="A21" s="38"/>
       <c r="B21" s="92" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C21" s="92"/>
       <c r="D21" s="92"/>
@@ -6878,10 +6584,10 @@
     <row r="22" spans="1:4" ht="20.25">
       <c r="A22" s="38"/>
       <c r="B22" s="92" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22" s="93" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D22" s="92"/>
     </row>
@@ -6893,7 +6599,7 @@
     </row>
     <row r="24" spans="1:4" ht="21">
       <c r="A24" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B24" s="92"/>
       <c r="C24" s="92"/>
@@ -6902,14 +6608,14 @@
     <row r="25" spans="1:4" ht="76.5">
       <c r="A25" s="4"/>
       <c r="B25" s="94" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C25" s="92"/>
       <c r="D25" s="92"/>
     </row>
     <row r="26" spans="1:4" ht="60">
       <c r="B26" s="94" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="48.75" customHeight="1">
@@ -6990,22 +6696,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75">
       <c r="A1" s="88" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="18.75">
       <c r="A20" s="88" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -7162,7 +6868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -7217,13 +6923,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="100" t="s">
         <v>192</v>
       </c>
-      <c r="C5" s="100" t="s">
-        <v>193</v>
-      </c>
       <c r="D5" s="103" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -7234,7 +6940,7 @@
         <v>59</v>
       </c>
       <c r="E9" s="64" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F9" s="65" t="s">
         <v>59</v>
@@ -7252,7 +6958,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="B12" s="67" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C12" s="66"/>
       <c r="G12" s="59"/>
@@ -7269,13 +6975,13 @@
     </row>
     <row r="15" spans="1:7">
       <c r="B15" s="113" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C15" s="114"/>
     </row>
     <row r="16" spans="1:7">
       <c r="B16" s="115" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C16" s="116"/>
     </row>
@@ -7293,22 +6999,22 @@
     </row>
     <row r="19" spans="1:8" ht="15.75">
       <c r="A19" s="33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B19" s="64" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D19" s="65" t="s">
         <v>59</v>
       </c>
       <c r="F19" s="67" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" s="95" t="s">
         <v>159</v>
-      </c>
-      <c r="G19" s="95" t="s">
-        <v>160</v>
       </c>
       <c r="H19" s="66" t="s">
         <v>59</v>
@@ -7332,62 +7038,62 @@
     </row>
     <row r="23" spans="1:8">
       <c r="B23" s="108" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C23" s="108" t="s">
         <v>59</v>
       </c>
       <c r="D23" s="108" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F23" s="109" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G23" s="109" t="s">
         <v>59</v>
       </c>
       <c r="H23" s="109" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="B24" s="108" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C24" s="108" t="s">
         <v>59</v>
       </c>
       <c r="D24" s="108" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F24" s="109" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G24" s="109" t="s">
         <v>59</v>
       </c>
       <c r="H24" s="109" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" s="108" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C25" s="108" t="s">
         <v>59</v>
       </c>
       <c r="D25" s="108" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F25" s="109" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G25" s="109" t="s">
         <v>59</v>
       </c>
       <c r="H25" s="109" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="21">
@@ -7406,10 +7112,10 @@
     </row>
     <row r="31" spans="1:8">
       <c r="B31" s="128" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" s="131" t="s">
         <v>157</v>
-      </c>
-      <c r="C31" s="131" t="s">
-        <v>158</v>
       </c>
       <c r="D31" s="132"/>
     </row>
@@ -7471,27 +7177,27 @@
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
       <c r="D4" s="101" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E4" s="102" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1">
       <c r="B5" s="117" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C5" s="118" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D5" s="104" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E5" s="105" t="s">
         <v>64</v>
       </c>
       <c r="F5" s="106" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G5" s="107" t="s">
         <v>65</v>
@@ -7527,33 +7233,33 @@
     </row>
     <row r="12" spans="1:9">
       <c r="B12" s="112" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="63" t="s">
         <v>175</v>
       </c>
-      <c r="C12" s="63" t="s">
-        <v>176</v>
-      </c>
       <c r="E12" s="110" t="s">
+        <v>163</v>
+      </c>
+      <c r="F12" s="110" t="s">
         <v>164</v>
       </c>
-      <c r="F12" s="110" t="s">
-        <v>165</v>
-      </c>
       <c r="H12" s="111" t="s">
+        <v>163</v>
+      </c>
+      <c r="I12" s="111" t="s">
         <v>164</v>
-      </c>
-      <c r="I12" s="111" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="B13" s="63"/>
       <c r="C13" s="63"/>
       <c r="E13" s="110" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F13" s="110"/>
       <c r="H13" s="111" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I13" s="111"/>
     </row>
@@ -7674,7 +7380,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="85" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B8" t="s">
         <v>93</v>
@@ -7694,10 +7400,10 @@
     </row>
     <row r="11" spans="1:8" ht="21">
       <c r="A11" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="85" t="s">
         <v>179</v>
-      </c>
-      <c r="B11" s="85" t="s">
-        <v>180</v>
       </c>
       <c r="C11">
         <f>SUM(TestRange1)</f>
@@ -7705,7 +7411,7 @@
       </c>
       <c r="D11" s="59"/>
       <c r="F11" s="85" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G11">
         <f>SUM(RangeMerged,F14:H14)</f>
@@ -7776,7 +7482,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7801,7 +7507,7 @@
     <row r="2" spans="1:3" ht="31.5">
       <c r="A2" s="86"/>
       <c r="B2" s="87" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2">
         <f>SUM([1]Sheet1!$A$3:$C$4)</f>
@@ -7814,10 +7520,10 @@
     </row>
     <row r="4" spans="1:3" ht="61.5">
       <c r="A4" s="86" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" s="87" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C4" t="str">
         <f>row!A1</f>
@@ -7826,7 +7532,7 @@
     </row>
     <row r="5" spans="1:3" ht="45">
       <c r="B5" s="87" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5">
         <f>SUM('cell-data'!F14:H14)</f>
@@ -7854,34 +7560,34 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="21">
       <c r="A2" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="21">
       <c r="A3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:13" hidden="1"/>
@@ -7907,55 +7613,55 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -7982,28 +7688,28 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="C1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="C2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="61.5" customHeight="1">
       <c r="A3" s="84" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" s="84" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="C5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:3" hidden="1"/>
@@ -8016,8 +7722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N249"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="F168" sqref="F168"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="L136" sqref="L136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8396,12 +8102,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="136" spans="1:12">
-      <c r="L136" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="137" spans="1:12" ht="18.75">
+    <row r="137" spans="1:1" ht="18.75">
       <c r="A137" s="88" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
* rename "XSheet sheet" to "XSheet xsheet" * add a variable "Sheet sheet"
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="cell-text" sheetId="1" r:id="rId1"/>
@@ -1819,6 +1819,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:view3D>
       <c:rotX val="30"/>
@@ -3135,6 +3136,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3418,6 +3420,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3449,6 +3452,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3811,6 +3815,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -4090,6 +4095,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -4373,6 +4379,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -4661,6 +4668,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -4935,6 +4943,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -5225,6 +5234,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -6313,8 +6323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6688,7 +6698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -7722,8 +7732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="L136" sqref="L136"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="L148" sqref="L148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add a bubble chart for test
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="196">
   <si>
     <t>autofilter</t>
   </si>
@@ -616,6 +616,15 @@
   </si>
   <si>
     <t>dotted</t>
+  </si>
+  <si>
+    <t>Number of Products</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Market Share</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1550,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1748,6 +1757,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1763,6 +1775,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1819,7 +1833,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:view3D>
       <c:rotX val="30"/>
@@ -1922,7 +1935,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1942,10 +1955,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15789749537121886"/>
+          <c:x val="0.15789749537121892"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.58796850393700595"/>
-          <c:h val="0.76578566465956754"/>
+          <c:w val="0.58796850393700573"/>
+          <c:h val="0.76578566465956777"/>
         </c:manualLayout>
       </c:layout>
       <c:area3DChart>
@@ -2172,25 +2185,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="60948864"/>
-        <c:axId val="60950400"/>
-        <c:axId val="96341504"/>
+        <c:axId val="95131520"/>
+        <c:axId val="95133056"/>
+        <c:axId val="93314112"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="60948864"/>
+        <c:axId val="95131520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60950400"/>
+        <c:crossAx val="95133056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60950400"/>
+        <c:axId val="95133056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2198,18 +2211,18 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60948864"/>
+        <c:crossAx val="95131520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="96341504"/>
+        <c:axId val="93314112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60950400"/>
+        <c:crossAx val="95133056"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2224,7 +2237,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2475,22 +2488,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="60960768"/>
-        <c:axId val="60962304"/>
+        <c:axId val="100689408"/>
+        <c:axId val="100690944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60960768"/>
+        <c:axId val="100689408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60962304"/>
+        <c:crossAx val="100690944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60962304"/>
+        <c:axId val="100690944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2498,7 +2511,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60960768"/>
+        <c:crossAx val="100689408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2511,7 +2524,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2774,13 +2787,140 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:bubbleChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'chart-image'!$A$159:$A$163</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'chart-image'!$B$159:$B$163</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'chart-image'!$C$159:$C$163</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+        </c:ser>
+        <c:bubbleScale val="100"/>
+        <c:axId val="113941504"/>
+        <c:axId val="113939200"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="113941504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113939200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="113939200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113941504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3106,22 +3246,22 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="75749248"/>
-        <c:axId val="75750784"/>
+        <c:axId val="101032320"/>
+        <c:axId val="101033856"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="75749248"/>
+        <c:axId val="101032320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75750784"/>
+        <c:crossAx val="101033856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75750784"/>
+        <c:axId val="101033856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3129,26 +3269,25 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75749248"/>
+        <c:crossAx val="101032320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3387,25 +3526,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="75862400"/>
-        <c:axId val="75863936"/>
+        <c:axId val="101128832"/>
+        <c:axId val="101134720"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="75862400"/>
+        <c:axId val="101128832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75863936"/>
+        <c:crossAx val="101134720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75863936"/>
+        <c:axId val="101134720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3413,20 +3552,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75862400"/>
+        <c:crossAx val="101128832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3452,7 +3590,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3526,8 +3663,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.70019920318725093"/>
           <c:y val="0.18529458333168791"/>
-          <c:w val="0.25885988970479895"/>
-          <c:h val="0.56509104330708848"/>
+          <c:w val="0.25885988970479901"/>
+          <c:h val="0.5650910433070887"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -3546,7 +3683,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3783,24 +3920,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="90990080"/>
-        <c:axId val="91384064"/>
+        <c:axId val="92514944"/>
+        <c:axId val="92524928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90990080"/>
+        <c:axId val="92514944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91384064"/>
+        <c:crossAx val="92524928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91384064"/>
+        <c:axId val="92524928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3808,20 +3945,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90990080"/>
+        <c:crossAx val="92514944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4062,25 +4198,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="95118080"/>
-        <c:axId val="95151232"/>
+        <c:axId val="92800512"/>
+        <c:axId val="92802048"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="95118080"/>
+        <c:axId val="92800512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95151232"/>
+        <c:crossAx val="92802048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95151232"/>
+        <c:axId val="92802048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4088,20 +4224,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95118080"/>
+        <c:crossAx val="92800512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4347,24 +4482,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="124593280"/>
-        <c:axId val="124596992"/>
+        <c:axId val="92831744"/>
+        <c:axId val="92833280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="124593280"/>
+        <c:axId val="92831744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124596992"/>
+        <c:crossAx val="92833280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124596992"/>
+        <c:axId val="92833280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4372,20 +4507,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124593280"/>
+        <c:crossAx val="92831744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4624,25 +4758,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="58766464"/>
-        <c:axId val="58768000"/>
-        <c:axId val="78172608"/>
+        <c:axId val="93596288"/>
+        <c:axId val="93602176"/>
+        <c:axId val="92854016"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="58766464"/>
+        <c:axId val="93596288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58768000"/>
+        <c:crossAx val="93602176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58768000"/>
+        <c:axId val="93602176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4650,31 +4784,30 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58766464"/>
+        <c:crossAx val="93596288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="78172608"/>
+        <c:axId val="92854016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="58768000"/>
+        <c:crossAx val="93602176"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4911,24 +5044,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="58782464"/>
-        <c:axId val="58784000"/>
+        <c:axId val="93640960"/>
+        <c:axId val="93261824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58782464"/>
+        <c:axId val="93640960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58784000"/>
+        <c:crossAx val="93261824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58784000"/>
+        <c:axId val="93261824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4936,20 +5069,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58782464"/>
+        <c:crossAx val="93640960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4971,7 +5103,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.25918955252544651"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.50321397186770456"/>
+          <c:w val="0.50321397186770445"/>
           <c:h val="0.8221582606228276"/>
         </c:manualLayout>
       </c:layout>
@@ -5201,25 +5333,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="60546432"/>
-        <c:axId val="60699776"/>
+        <c:axId val="93287936"/>
+        <c:axId val="93289472"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="60546432"/>
+        <c:axId val="93287936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60699776"/>
+        <c:crossAx val="93289472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60699776"/>
+        <c:axId val="93289472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5227,14 +5359,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60546432"/>
+        <c:crossAx val="93287936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -5243,7 +5374,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5479,24 +5610,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="60729216"/>
-        <c:axId val="60730752"/>
+        <c:axId val="93318528"/>
+        <c:axId val="95093888"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="60729216"/>
+        <c:axId val="93318528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60730752"/>
+        <c:crossAx val="95093888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60730752"/>
+        <c:axId val="95093888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5504,7 +5635,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60729216"/>
+        <c:crossAx val="93318528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5517,7 +5648,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5922,6 +6053,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="20" name="Chart 19"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6366,17 +6527,17 @@
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="124" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="124"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
@@ -6448,17 +6609,17 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="125" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="124"/>
-      <c r="F6" s="124"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="124"/>
-      <c r="J6" s="124"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="125"/>
+      <c r="J6" s="125"/>
     </row>
     <row r="7" spans="1:13" ht="92.25">
       <c r="A7" s="23" t="s">
@@ -6849,13 +7010,13 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="125" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
@@ -7110,34 +7271,34 @@
       <c r="A28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="125" t="s">
+      <c r="B28" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="126"/>
-      <c r="E28" s="125" t="s">
+      <c r="C28" s="127"/>
+      <c r="E28" s="126" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="127"/>
-      <c r="G28" s="126"/>
+      <c r="F28" s="128"/>
+      <c r="G28" s="127"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="128" t="s">
+      <c r="B31" s="129" t="s">
         <v>156</v>
       </c>
-      <c r="C31" s="131" t="s">
+      <c r="C31" s="132" t="s">
         <v>157</v>
       </c>
-      <c r="D31" s="132"/>
+      <c r="D31" s="133"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="129"/>
-      <c r="C32" s="133"/>
-      <c r="D32" s="134"/>
+      <c r="B32" s="130"/>
+      <c r="C32" s="134"/>
+      <c r="D32" s="135"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="130"/>
-      <c r="C33" s="135"/>
-      <c r="D33" s="136"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="136"/>
+      <c r="D33" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -7438,11 +7599,11 @@
       <c r="D12" s="65">
         <v>3</v>
       </c>
-      <c r="F12" s="131">
+      <c r="F12" s="132">
         <v>1</v>
       </c>
-      <c r="G12" s="137"/>
-      <c r="H12" s="132"/>
+      <c r="G12" s="138"/>
+      <c r="H12" s="133"/>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" s="66">
@@ -7454,9 +7615,9 @@
       <c r="D13" s="67">
         <v>6</v>
       </c>
-      <c r="F13" s="135"/>
-      <c r="G13" s="138"/>
-      <c r="H13" s="136"/>
+      <c r="F13" s="136"/>
+      <c r="G13" s="139"/>
+      <c r="H13" s="137"/>
     </row>
     <row r="14" spans="1:8">
       <c r="F14">
@@ -7732,14 +7893,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="L148" sqref="L148"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21">
@@ -8115,6 +8277,77 @@
     <row r="137" spans="1:1" ht="18.75">
       <c r="A137" s="88" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="18.75">
+      <c r="A155" s="88" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="30">
+      <c r="A158" t="s">
+        <v>193</v>
+      </c>
+      <c r="B158" t="s">
+        <v>194</v>
+      </c>
+      <c r="C158" s="123" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159">
+        <v>5</v>
+      </c>
+      <c r="B159" s="141">
+        <v>5500</v>
+      </c>
+      <c r="C159" s="140">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160">
+        <v>14</v>
+      </c>
+      <c r="B160" s="141">
+        <v>12200</v>
+      </c>
+      <c r="C160" s="140">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161">
+        <v>20</v>
+      </c>
+      <c r="B161" s="141">
+        <v>60000</v>
+      </c>
+      <c r="C161" s="140">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162">
+        <v>18</v>
+      </c>
+      <c r="B162" s="141">
+        <v>24400</v>
+      </c>
+      <c r="C162" s="140">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163">
+        <v>22</v>
+      </c>
+      <c r="B163" s="141">
+        <v>32000</v>
+      </c>
+      <c r="C163" s="140">
+        <v>0.42</v>
       </c>
     </row>
     <row r="249" spans="1:1" ht="21">
@@ -8139,6 +8372,7 @@
     <hyperlink ref="A14" r:id="rId15" location="browser-ww-monthly-201201-201201-bar" display="http://gs.statcounter.com/ - browser-ww-monthly-201201-201201-bar"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId16"/>
+  <drawing r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change test Excel file's protection configuration. In "Format Cells..." , uncheck "lock" option. This is what Spreadsheet supports.
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="cell-text" sheetId="1" r:id="rId1"/>
@@ -1550,7 +1550,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1757,6 +1757,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1775,8 +1777,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1803,6 +1806,72 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FFFF0000"/>
       <color rgb="FF0000FF"/>
@@ -1935,7 +2004,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1955,10 +2024,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15789749537121892"/>
+          <c:x val="0.15789749537121897"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.58796850393700573"/>
-          <c:h val="0.76578566465956777"/>
+          <c:w val="0.5879685039370055"/>
+          <c:h val="0.76578566465956799"/>
         </c:manualLayout>
       </c:layout>
       <c:area3DChart>
@@ -2185,25 +2254,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="95131520"/>
-        <c:axId val="95133056"/>
-        <c:axId val="93314112"/>
+        <c:axId val="69651840"/>
+        <c:axId val="69657728"/>
+        <c:axId val="83910656"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="95131520"/>
+        <c:axId val="69651840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95133056"/>
+        <c:crossAx val="69657728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95133056"/>
+        <c:axId val="69657728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2211,24 +2280,23 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95131520"/>
+        <c:crossAx val="69651840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="93314112"/>
+        <c:axId val="83910656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95133056"/>
+        <c:crossAx val="69657728"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2237,7 +2305,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2488,22 +2556,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="100689408"/>
-        <c:axId val="100690944"/>
+        <c:axId val="83921920"/>
+        <c:axId val="85447424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100689408"/>
+        <c:axId val="83921920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100690944"/>
+        <c:crossAx val="85447424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100690944"/>
+        <c:axId val="85447424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2511,20 +2579,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100689408"/>
+        <c:crossAx val="83921920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2787,7 +2854,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2877,23 +2944,23 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="113941504"/>
-        <c:axId val="113939200"/>
+        <c:axId val="85753216"/>
+        <c:axId val="85755008"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="113941504"/>
+        <c:axId val="85753216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113939200"/>
+        <c:crossAx val="85755008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113939200"/>
+        <c:axId val="85755008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2901,7 +2968,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113941504"/>
+        <c:crossAx val="85753216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2914,7 +2981,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3246,22 +3313,22 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="101032320"/>
-        <c:axId val="101033856"/>
+        <c:axId val="85818368"/>
+        <c:axId val="85820160"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="101032320"/>
+        <c:axId val="85818368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101033856"/>
+        <c:crossAx val="85820160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101033856"/>
+        <c:axId val="85820160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3269,19 +3336,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101032320"/>
+        <c:crossAx val="85818368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3526,25 +3594,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="101128832"/>
-        <c:axId val="101134720"/>
+        <c:axId val="85845504"/>
+        <c:axId val="85847040"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="101128832"/>
+        <c:axId val="85845504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101134720"/>
+        <c:crossAx val="85847040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101134720"/>
+        <c:axId val="85847040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3552,19 +3620,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101128832"/>
+        <c:crossAx val="85845504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3663,8 +3732,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.70019920318725093"/>
           <c:y val="0.18529458333168791"/>
-          <c:w val="0.25885988970479901"/>
-          <c:h val="0.5650910433070887"/>
+          <c:w val="0.25885988970479906"/>
+          <c:h val="0.56509104330708881"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -3683,7 +3752,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3920,24 +3989,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="92514944"/>
-        <c:axId val="92524928"/>
+        <c:axId val="69497216"/>
+        <c:axId val="69498752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92514944"/>
+        <c:axId val="69497216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92524928"/>
+        <c:crossAx val="69498752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92524928"/>
+        <c:axId val="69498752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3945,7 +4014,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92514944"/>
+        <c:crossAx val="69497216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3957,7 +4026,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4198,25 +4267,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="92800512"/>
-        <c:axId val="92802048"/>
+        <c:axId val="69508096"/>
+        <c:axId val="69526272"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="92800512"/>
+        <c:axId val="69508096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92802048"/>
+        <c:crossAx val="69526272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92802048"/>
+        <c:axId val="69526272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4224,7 +4293,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92800512"/>
+        <c:crossAx val="69508096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4236,7 +4305,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4482,24 +4551,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92831744"/>
-        <c:axId val="92833280"/>
+        <c:axId val="69539328"/>
+        <c:axId val="69540864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92831744"/>
+        <c:axId val="69539328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92833280"/>
+        <c:crossAx val="69540864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92833280"/>
+        <c:axId val="69540864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4507,7 +4576,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92831744"/>
+        <c:crossAx val="69539328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4519,7 +4588,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4758,25 +4827,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="93596288"/>
-        <c:axId val="93602176"/>
-        <c:axId val="92854016"/>
+        <c:axId val="69562752"/>
+        <c:axId val="69564288"/>
+        <c:axId val="99521408"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="93596288"/>
+        <c:axId val="69562752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93602176"/>
+        <c:crossAx val="69564288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93602176"/>
+        <c:axId val="69564288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4784,19 +4853,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93596288"/>
+        <c:crossAx val="69562752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="92854016"/>
+        <c:axId val="99521408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="93602176"/>
+        <c:crossAx val="69564288"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -4807,7 +4876,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5044,24 +5113,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="93640960"/>
-        <c:axId val="93261824"/>
+        <c:axId val="69582848"/>
+        <c:axId val="69584384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93640960"/>
+        <c:axId val="69582848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93261824"/>
+        <c:crossAx val="69584384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93261824"/>
+        <c:axId val="69584384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5069,7 +5138,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93640960"/>
+        <c:crossAx val="69582848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5081,7 +5150,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5103,7 +5172,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.25918955252544651"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.50321397186770445"/>
+          <c:w val="0.50321397186770422"/>
           <c:h val="0.8221582606228276"/>
         </c:manualLayout>
       </c:layout>
@@ -5333,25 +5402,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="93287936"/>
-        <c:axId val="93289472"/>
+        <c:axId val="69606400"/>
+        <c:axId val="69616384"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="93287936"/>
+        <c:axId val="69606400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93289472"/>
+        <c:crossAx val="69616384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93289472"/>
+        <c:axId val="69616384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5359,7 +5428,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93287936"/>
+        <c:crossAx val="69606400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5374,7 +5443,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5610,24 +5679,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="93318528"/>
-        <c:axId val="95093888"/>
+        <c:axId val="69629056"/>
+        <c:axId val="69630592"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="93318528"/>
+        <c:axId val="69629056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95093888"/>
+        <c:crossAx val="69630592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95093888"/>
+        <c:axId val="69630592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5635,20 +5704,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93318528"/>
+        <c:crossAx val="69629056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6205,7 +6273,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -6527,17 +6595,17 @@
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
@@ -6609,17 +6677,17 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="127" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
-      <c r="G6" s="125"/>
-      <c r="H6" s="125"/>
-      <c r="I6" s="125"/>
-      <c r="J6" s="125"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
     </row>
     <row r="7" spans="1:13" ht="92.25">
       <c r="A7" s="23" t="s">
@@ -7003,31 +7071,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="127" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" s="142" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A2" name="AllowableTest"/>
-  </protectedRanges>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
@@ -7271,34 +7339,34 @@
       <c r="A28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="126" t="s">
+      <c r="B28" s="128" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="127"/>
-      <c r="E28" s="126" t="s">
+      <c r="C28" s="129"/>
+      <c r="E28" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="128"/>
-      <c r="G28" s="127"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="129"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="129" t="s">
+      <c r="B31" s="131" t="s">
         <v>156</v>
       </c>
-      <c r="C31" s="132" t="s">
+      <c r="C31" s="134" t="s">
         <v>157</v>
       </c>
-      <c r="D31" s="133"/>
+      <c r="D31" s="135"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="130"/>
-      <c r="C32" s="134"/>
-      <c r="D32" s="135"/>
+      <c r="B32" s="132"/>
+      <c r="C32" s="136"/>
+      <c r="D32" s="137"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="131"/>
-      <c r="C33" s="136"/>
-      <c r="D33" s="137"/>
+      <c r="B33" s="133"/>
+      <c r="C33" s="138"/>
+      <c r="D33" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -7599,11 +7667,11 @@
       <c r="D12" s="65">
         <v>3</v>
       </c>
-      <c r="F12" s="132">
+      <c r="F12" s="134">
         <v>1</v>
       </c>
-      <c r="G12" s="138"/>
-      <c r="H12" s="133"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="135"/>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" s="66">
@@ -7615,9 +7683,9 @@
       <c r="D13" s="67">
         <v>6</v>
       </c>
-      <c r="F13" s="136"/>
-      <c r="G13" s="139"/>
-      <c r="H13" s="137"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="141"/>
+      <c r="H13" s="139"/>
     </row>
     <row r="14" spans="1:8">
       <c r="F14">
@@ -7893,7 +7961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+    <sheetView topLeftCell="A143" workbookViewId="0">
       <selection activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
@@ -8299,10 +8367,10 @@
       <c r="A159">
         <v>5</v>
       </c>
-      <c r="B159" s="141">
+      <c r="B159" s="125">
         <v>5500</v>
       </c>
-      <c r="C159" s="140">
+      <c r="C159" s="124">
         <v>0.03</v>
       </c>
     </row>
@@ -8310,10 +8378,10 @@
       <c r="A160">
         <v>14</v>
       </c>
-      <c r="B160" s="141">
+      <c r="B160" s="125">
         <v>12200</v>
       </c>
-      <c r="C160" s="140">
+      <c r="C160" s="124">
         <v>0.12</v>
       </c>
     </row>
@@ -8321,10 +8389,10 @@
       <c r="A161">
         <v>20</v>
       </c>
-      <c r="B161" s="141">
+      <c r="B161" s="125">
         <v>60000</v>
       </c>
-      <c r="C161" s="140">
+      <c r="C161" s="124">
         <v>0.33</v>
       </c>
     </row>
@@ -8332,10 +8400,10 @@
       <c r="A162">
         <v>18</v>
       </c>
-      <c r="B162" s="141">
+      <c r="B162" s="125">
         <v>24400</v>
       </c>
-      <c r="C162" s="140">
+      <c r="C162" s="124">
         <v>0.1</v>
       </c>
     </row>
@@ -8343,10 +8411,10 @@
       <c r="A163">
         <v>22</v>
       </c>
-      <c r="B163" s="141">
+      <c r="B163" s="125">
         <v>32000</v>
       </c>
-      <c r="C163" s="140">
+      <c r="C163" s="124">
         <v>0.42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix validation settings of TestFile2003.xls, TestFile2007.xlsx
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cell-text" sheetId="1" r:id="rId1"/>
@@ -1759,6 +1759,9 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1777,9 +1780,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2004,7 +2004,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2024,10 +2024,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15789749537121897"/>
+          <c:x val="0.15789749537121903"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.5879685039370055"/>
-          <c:h val="0.76578566465956799"/>
+          <c:w val="0.58796850393700539"/>
+          <c:h val="0.76578566465956821"/>
         </c:manualLayout>
       </c:layout>
       <c:area3DChart>
@@ -2254,25 +2254,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="69651840"/>
-        <c:axId val="69657728"/>
-        <c:axId val="83910656"/>
+        <c:axId val="69653248"/>
+        <c:axId val="69654784"/>
+        <c:axId val="69611008"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="69651840"/>
+        <c:axId val="69653248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69657728"/>
+        <c:crossAx val="69654784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69657728"/>
+        <c:axId val="69654784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2280,18 +2280,18 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69651840"/>
+        <c:crossAx val="69653248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="83910656"/>
+        <c:axId val="69611008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69657728"/>
+        <c:crossAx val="69654784"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2305,7 +2305,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2556,22 +2556,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="83921920"/>
-        <c:axId val="85447424"/>
+        <c:axId val="70545792"/>
+        <c:axId val="70547328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83921920"/>
+        <c:axId val="70545792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85447424"/>
+        <c:crossAx val="70547328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85447424"/>
+        <c:axId val="70547328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2579,7 +2579,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83921920"/>
+        <c:crossAx val="70545792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2591,7 +2591,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2848,13 +2848,12 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2944,23 +2943,23 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="85753216"/>
-        <c:axId val="85755008"/>
+        <c:axId val="70611712"/>
+        <c:axId val="70613248"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="85753216"/>
+        <c:axId val="70611712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85755008"/>
+        <c:crossAx val="70613248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85755008"/>
+        <c:axId val="70613248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2968,20 +2967,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85753216"/>
+        <c:crossAx val="70611712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3313,22 +3311,22 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="85818368"/>
-        <c:axId val="85820160"/>
+        <c:axId val="83345792"/>
+        <c:axId val="83347328"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="85818368"/>
+        <c:axId val="83345792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85820160"/>
+        <c:crossAx val="83347328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85820160"/>
+        <c:axId val="83347328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3336,20 +3334,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85818368"/>
+        <c:crossAx val="83345792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3594,25 +3591,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="85845504"/>
-        <c:axId val="85847040"/>
+        <c:axId val="83921536"/>
+        <c:axId val="85004672"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="85845504"/>
+        <c:axId val="83921536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85847040"/>
+        <c:crossAx val="85004672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85847040"/>
+        <c:axId val="85004672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3620,20 +3617,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85845504"/>
+        <c:crossAx val="83921536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3732,8 +3728,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.70019920318725093"/>
           <c:y val="0.18529458333168791"/>
-          <c:w val="0.25885988970479906"/>
-          <c:h val="0.56509104330708881"/>
+          <c:w val="0.25885988970479912"/>
+          <c:h val="0.56509104330708892"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -3752,7 +3748,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3989,24 +3985,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="69497216"/>
-        <c:axId val="69498752"/>
+        <c:axId val="100435840"/>
+        <c:axId val="100437376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="69497216"/>
+        <c:axId val="100435840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69498752"/>
+        <c:crossAx val="100437376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69498752"/>
+        <c:axId val="100437376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4014,7 +4010,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69497216"/>
+        <c:crossAx val="100435840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4026,7 +4022,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4267,25 +4263,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="69508096"/>
-        <c:axId val="69526272"/>
+        <c:axId val="69468544"/>
+        <c:axId val="69470080"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="69508096"/>
+        <c:axId val="69468544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69526272"/>
+        <c:crossAx val="69470080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69526272"/>
+        <c:axId val="69470080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4293,7 +4289,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69508096"/>
+        <c:crossAx val="69468544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4305,7 +4301,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4551,24 +4547,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="69539328"/>
-        <c:axId val="69540864"/>
+        <c:axId val="69491328"/>
+        <c:axId val="69501312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69539328"/>
+        <c:axId val="69491328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69540864"/>
+        <c:crossAx val="69501312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69540864"/>
+        <c:axId val="69501312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4576,7 +4572,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69539328"/>
+        <c:crossAx val="69491328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4588,7 +4584,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4827,25 +4823,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="69562752"/>
-        <c:axId val="69564288"/>
-        <c:axId val="99521408"/>
+        <c:axId val="69514752"/>
+        <c:axId val="69516288"/>
+        <c:axId val="69478592"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="69562752"/>
+        <c:axId val="69514752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69564288"/>
+        <c:crossAx val="69516288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69564288"/>
+        <c:axId val="69516288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4853,19 +4849,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69562752"/>
+        <c:crossAx val="69514752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="99521408"/>
+        <c:axId val="69478592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="69564288"/>
+        <c:crossAx val="69516288"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -4876,7 +4872,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5113,24 +5109,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="69582848"/>
-        <c:axId val="69584384"/>
+        <c:axId val="69551232"/>
+        <c:axId val="69552768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="69582848"/>
+        <c:axId val="69551232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69584384"/>
+        <c:crossAx val="69552768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69584384"/>
+        <c:axId val="69552768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5138,7 +5134,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69582848"/>
+        <c:crossAx val="69551232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5150,7 +5146,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5172,7 +5168,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.25918955252544651"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.50321397186770422"/>
+          <c:w val="0.503213971867704"/>
           <c:h val="0.8221582606228276"/>
         </c:manualLayout>
       </c:layout>
@@ -5402,25 +5398,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="69606400"/>
-        <c:axId val="69616384"/>
+        <c:axId val="69587328"/>
+        <c:axId val="69588864"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="69606400"/>
+        <c:axId val="69587328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69616384"/>
+        <c:crossAx val="69588864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69616384"/>
+        <c:axId val="69588864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5428,7 +5424,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69606400"/>
+        <c:crossAx val="69587328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5443,7 +5439,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5679,24 +5675,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="69629056"/>
-        <c:axId val="69630592"/>
+        <c:axId val="69601536"/>
+        <c:axId val="69640192"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="69629056"/>
+        <c:axId val="69601536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69630592"/>
+        <c:crossAx val="69640192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69630592"/>
+        <c:axId val="69640192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5704,7 +5700,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69629056"/>
+        <c:crossAx val="69601536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5716,7 +5712,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6595,17 +6591,17 @@
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="126" t="s">
+      <c r="B3" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="126"/>
-      <c r="J3" s="126"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="127"/>
+      <c r="J3" s="127"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
@@ -6677,17 +6673,17 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="127" t="s">
+      <c r="B6" s="128" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="128"/>
     </row>
     <row r="7" spans="1:13" ht="92.25">
       <c r="A7" s="23" t="s">
@@ -7071,7 +7067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -7081,16 +7077,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="128" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="126" t="s">
         <v>69</v>
       </c>
     </row>
@@ -7339,34 +7335,34 @@
       <c r="A28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="128" t="s">
+      <c r="B28" s="129" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="129"/>
-      <c r="E28" s="128" t="s">
+      <c r="C28" s="130"/>
+      <c r="E28" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="130"/>
-      <c r="G28" s="129"/>
+      <c r="F28" s="131"/>
+      <c r="G28" s="130"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="131" t="s">
+      <c r="B31" s="132" t="s">
         <v>156</v>
       </c>
-      <c r="C31" s="134" t="s">
+      <c r="C31" s="135" t="s">
         <v>157</v>
       </c>
-      <c r="D31" s="135"/>
+      <c r="D31" s="136"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="132"/>
-      <c r="C32" s="136"/>
-      <c r="D32" s="137"/>
+      <c r="B32" s="133"/>
+      <c r="C32" s="137"/>
+      <c r="D32" s="138"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="133"/>
-      <c r="C33" s="138"/>
-      <c r="D33" s="139"/>
+      <c r="B33" s="134"/>
+      <c r="C33" s="139"/>
+      <c r="D33" s="140"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -7518,8 +7514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7667,11 +7663,11 @@
       <c r="D12" s="65">
         <v>3</v>
       </c>
-      <c r="F12" s="134">
+      <c r="F12" s="135">
         <v>1</v>
       </c>
-      <c r="G12" s="140"/>
-      <c r="H12" s="135"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="136"/>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" s="66">
@@ -7683,9 +7679,9 @@
       <c r="D13" s="67">
         <v>6</v>
       </c>
-      <c r="F13" s="138"/>
-      <c r="G13" s="141"/>
-      <c r="H13" s="139"/>
+      <c r="F13" s="139"/>
+      <c r="G13" s="142"/>
+      <c r="H13" s="140"/>
     </row>
     <row r="14" spans="1:8">
       <c r="F14">
@@ -7702,9 +7698,9 @@
   <mergeCells count="1">
     <mergeCell ref="F12:H13"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid grade" error="not a valid grade" promptTitle="4 grades only" prompt="input a grade score" sqref="B8">
-      <formula1>$C$88:$F$88</formula1>
+      <formula1>$C$8:$F$8</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sorry" error="1 - 10" prompt="valid between 1 to 10" sqref="B7">
       <formula1>1</formula1>

</xml_diff>

<commit_message>
change test file's sheet protection setting to that ZK spreadsheet can read.
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="cell-text" sheetId="1" r:id="rId1"/>
@@ -1035,7 +1035,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1533,6 +1533,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1541,7 +1556,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1763,6 +1778,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1789,6 +1807,72 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FFFF0000"/>
       <color rgb="FF0000FF"/>
@@ -1921,7 +2005,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1941,10 +2025,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15789749537121886"/>
+          <c:x val="0.15789749537121892"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.58796850393700595"/>
-          <c:h val="0.76578566465956754"/>
+          <c:w val="0.58796850393700573"/>
+          <c:h val="0.76578566465956777"/>
         </c:manualLayout>
       </c:layout>
       <c:area3DChart>
@@ -2171,25 +2255,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="60948864"/>
-        <c:axId val="60950400"/>
-        <c:axId val="96341504"/>
+        <c:axId val="70914432"/>
+        <c:axId val="70915968"/>
+        <c:axId val="70926336"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="60948864"/>
+        <c:axId val="70914432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60950400"/>
+        <c:crossAx val="70915968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60950400"/>
+        <c:axId val="70915968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2197,18 +2281,18 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60948864"/>
+        <c:crossAx val="70914432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="96341504"/>
+        <c:axId val="70926336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60950400"/>
+        <c:crossAx val="70915968"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2223,7 +2307,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2474,22 +2558,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="60960768"/>
-        <c:axId val="60962304"/>
+        <c:axId val="70950912"/>
+        <c:axId val="70952448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60960768"/>
+        <c:axId val="70950912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60962304"/>
+        <c:crossAx val="70952448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60962304"/>
+        <c:axId val="70952448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,7 +2581,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60960768"/>
+        <c:crossAx val="70950912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2510,7 +2594,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2767,13 +2851,12 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3105,22 +3188,22 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="75749248"/>
-        <c:axId val="75750784"/>
+        <c:axId val="71117440"/>
+        <c:axId val="71127424"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="75749248"/>
+        <c:axId val="71117440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75750784"/>
+        <c:crossAx val="71127424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75750784"/>
+        <c:axId val="71127424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3128,19 +3211,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75749248"/>
+        <c:crossAx val="71117440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3385,25 +3469,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="75862400"/>
-        <c:axId val="75863936"/>
+        <c:axId val="71152768"/>
+        <c:axId val="71154304"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="75862400"/>
+        <c:axId val="71152768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75863936"/>
+        <c:crossAx val="71154304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75863936"/>
+        <c:axId val="71154304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3411,19 +3495,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75862400"/>
+        <c:crossAx val="71152768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3522,8 +3607,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.70019920318725093"/>
           <c:y val="0.18529458333168791"/>
-          <c:w val="0.25885988970479895"/>
-          <c:h val="0.56509104330708848"/>
+          <c:w val="0.25885988970479901"/>
+          <c:h val="0.5650910433070887"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -3542,7 +3627,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3779,24 +3864,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="90990080"/>
-        <c:axId val="91384064"/>
+        <c:axId val="57500800"/>
+        <c:axId val="57502336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90990080"/>
+        <c:axId val="57500800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91384064"/>
+        <c:crossAx val="57502336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91384064"/>
+        <c:axId val="57502336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3804,7 +3889,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90990080"/>
+        <c:crossAx val="57500800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3816,7 +3901,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4057,25 +4142,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="95118080"/>
-        <c:axId val="95151232"/>
+        <c:axId val="57528320"/>
+        <c:axId val="57529856"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="95118080"/>
+        <c:axId val="57528320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95151232"/>
+        <c:crossAx val="57529856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95151232"/>
+        <c:axId val="57529856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4083,7 +4168,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95118080"/>
+        <c:crossAx val="57528320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4095,7 +4180,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4341,24 +4426,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="124593280"/>
-        <c:axId val="124596992"/>
+        <c:axId val="69605632"/>
+        <c:axId val="69611520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="124593280"/>
+        <c:axId val="69605632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124596992"/>
+        <c:crossAx val="69611520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124596992"/>
+        <c:axId val="69611520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4366,7 +4451,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124593280"/>
+        <c:crossAx val="69605632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4378,7 +4463,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4617,25 +4702,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="58766464"/>
-        <c:axId val="58768000"/>
-        <c:axId val="78172608"/>
+        <c:axId val="69649536"/>
+        <c:axId val="69651072"/>
+        <c:axId val="57526912"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="58766464"/>
+        <c:axId val="69649536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58768000"/>
+        <c:crossAx val="69651072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58768000"/>
+        <c:axId val="69651072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4643,19 +4728,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58766464"/>
+        <c:crossAx val="69649536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="78172608"/>
+        <c:axId val="57526912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="58768000"/>
+        <c:crossAx val="69651072"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -4666,7 +4751,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4903,24 +4988,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="58782464"/>
-        <c:axId val="58784000"/>
+        <c:axId val="69018368"/>
+        <c:axId val="69019904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58782464"/>
+        <c:axId val="69018368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58784000"/>
+        <c:crossAx val="69019904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58784000"/>
+        <c:axId val="69019904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4928,7 +5013,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58782464"/>
+        <c:crossAx val="69018368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4940,7 +5025,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4962,7 +5047,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.25918955252544651"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.50321397186770456"/>
+          <c:w val="0.50321397186770445"/>
           <c:h val="0.8221582606228276"/>
         </c:manualLayout>
       </c:layout>
@@ -5192,25 +5277,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="60546432"/>
-        <c:axId val="60699776"/>
+        <c:axId val="70193152"/>
+        <c:axId val="70194688"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="60546432"/>
+        <c:axId val="70193152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60699776"/>
+        <c:crossAx val="70194688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60699776"/>
+        <c:axId val="70194688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5218,7 +5303,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60546432"/>
+        <c:crossAx val="70193152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5233,7 +5318,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5469,24 +5554,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="60729216"/>
-        <c:axId val="60730752"/>
+        <c:axId val="70207360"/>
+        <c:axId val="70208896"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="60729216"/>
+        <c:axId val="70207360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60730752"/>
+        <c:crossAx val="70208896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60730752"/>
+        <c:axId val="70208896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5494,7 +5579,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60729216"/>
+        <c:crossAx val="70207360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5507,7 +5592,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6034,7 +6119,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -6830,13 +6915,16 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="124" t="s">
@@ -6847,20 +6935,19 @@
       <c r="D1" s="124"/>
       <c r="E1" s="124"/>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A3" s="139" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A2" name="AllowableTest"/>
-  </protectedRanges>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7722,7 +7809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="L136" sqref="L136"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
* fix ZSS-528. * modify test case to avoid misunderstanding.
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110"/>
   </bookViews>
   <sheets>
     <sheet name="cell-text" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="194">
   <si>
     <t>autofilter</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t>dotted</t>
+  </si>
+  <si>
+    <t>size 36</t>
   </si>
 </sst>
 </file>
@@ -820,14 +823,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="72"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -996,6 +991,14 @@
     <font>
       <u val="doubleAccounting"/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1551,7 +1554,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1618,37 +1621,34 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1677,7 +1677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -1692,7 +1692,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1708,22 +1708,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="45" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="44" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
@@ -1750,15 +1750,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1778,8 +1781,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1807,72 +1810,6 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FFFF0000"/>
       <color rgb="FF0000FF"/>
@@ -2005,7 +1942,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2025,10 +1962,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15789749537121892"/>
+          <c:x val="0.15789749537121903"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.58796850393700573"/>
-          <c:h val="0.76578566465956777"/>
+          <c:w val="0.58796850393700539"/>
+          <c:h val="0.76578566465956821"/>
         </c:manualLayout>
       </c:layout>
       <c:area3DChart>
@@ -2255,25 +2192,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="70914432"/>
-        <c:axId val="70915968"/>
-        <c:axId val="70926336"/>
+        <c:axId val="80718848"/>
+        <c:axId val="80732928"/>
+        <c:axId val="80697536"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="70914432"/>
+        <c:axId val="80718848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70915968"/>
+        <c:crossAx val="80732928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70915968"/>
+        <c:axId val="80732928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2281,24 +2218,23 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70914432"/>
+        <c:crossAx val="80718848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="70926336"/>
+        <c:axId val="80697536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70915968"/>
+        <c:crossAx val="80732928"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2307,7 +2243,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2558,22 +2494,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="70950912"/>
-        <c:axId val="70952448"/>
+        <c:axId val="88697472"/>
+        <c:axId val="88707456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70950912"/>
+        <c:axId val="88697472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70952448"/>
+        <c:crossAx val="88707456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70952448"/>
+        <c:axId val="88707456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2581,20 +2517,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70950912"/>
+        <c:crossAx val="88697472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2856,7 +2791,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3188,22 +3123,22 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="71117440"/>
-        <c:axId val="71127424"/>
+        <c:axId val="89814528"/>
+        <c:axId val="89816064"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="71117440"/>
+        <c:axId val="89814528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71127424"/>
+        <c:crossAx val="89816064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71127424"/>
+        <c:axId val="89816064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3211,20 +3146,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71117440"/>
+        <c:crossAx val="89814528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3469,25 +3403,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="71152768"/>
-        <c:axId val="71154304"/>
+        <c:axId val="91914240"/>
+        <c:axId val="91915776"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="71152768"/>
+        <c:axId val="91914240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71154304"/>
+        <c:crossAx val="91915776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71154304"/>
+        <c:axId val="91915776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3495,20 +3429,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71152768"/>
+        <c:crossAx val="91914240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3607,8 +3540,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.70019920318725093"/>
           <c:y val="0.18529458333168791"/>
-          <c:w val="0.25885988970479901"/>
-          <c:h val="0.5650910433070887"/>
+          <c:w val="0.25885988970479912"/>
+          <c:h val="0.56509104330708892"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -3627,7 +3560,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3864,24 +3797,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="57500800"/>
-        <c:axId val="57502336"/>
+        <c:axId val="78544896"/>
+        <c:axId val="78546432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57500800"/>
+        <c:axId val="78544896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57502336"/>
+        <c:crossAx val="78546432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57502336"/>
+        <c:axId val="78546432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3889,7 +3822,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57500800"/>
+        <c:crossAx val="78544896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3901,7 +3834,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4142,25 +4075,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="57528320"/>
-        <c:axId val="57529856"/>
+        <c:axId val="78576256"/>
+        <c:axId val="79671680"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="57528320"/>
+        <c:axId val="78576256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57529856"/>
+        <c:crossAx val="79671680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57529856"/>
+        <c:axId val="79671680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4168,7 +4101,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57528320"/>
+        <c:crossAx val="78576256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4180,7 +4113,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4426,24 +4359,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="69605632"/>
-        <c:axId val="69611520"/>
+        <c:axId val="80491648"/>
+        <c:axId val="80493184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69605632"/>
+        <c:axId val="80491648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69611520"/>
+        <c:crossAx val="80493184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69611520"/>
+        <c:axId val="80493184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4451,7 +4384,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69605632"/>
+        <c:crossAx val="80491648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4463,7 +4396,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4702,25 +4635,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="69649536"/>
-        <c:axId val="69651072"/>
-        <c:axId val="57526912"/>
+        <c:axId val="80547840"/>
+        <c:axId val="80549376"/>
+        <c:axId val="80507776"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="69649536"/>
+        <c:axId val="80547840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69651072"/>
+        <c:crossAx val="80549376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69651072"/>
+        <c:axId val="80549376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4728,19 +4661,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69649536"/>
+        <c:crossAx val="80547840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="57526912"/>
+        <c:axId val="80507776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="69651072"/>
+        <c:crossAx val="80549376"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -4751,7 +4684,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4988,24 +4921,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="69018368"/>
-        <c:axId val="69019904"/>
+        <c:axId val="80575872"/>
+        <c:axId val="80606336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="69018368"/>
+        <c:axId val="80575872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69019904"/>
+        <c:crossAx val="80606336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69019904"/>
+        <c:axId val="80606336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5013,7 +4946,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69018368"/>
+        <c:crossAx val="80575872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5025,7 +4958,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5047,7 +4980,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.25918955252544651"/>
           <c:y val="4.9549549549549488E-2"/>
-          <c:w val="0.50321397186770445"/>
+          <c:w val="0.503213971867704"/>
           <c:h val="0.8221582606228276"/>
         </c:manualLayout>
       </c:layout>
@@ -5277,25 +5210,25 @@
           </c:val>
         </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="70193152"/>
-        <c:axId val="70194688"/>
+        <c:axId val="80636544"/>
+        <c:axId val="80638336"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="70193152"/>
+        <c:axId val="80636544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70194688"/>
+        <c:crossAx val="80638336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70194688"/>
+        <c:axId val="80638336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5303,7 +5236,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70193152"/>
+        <c:crossAx val="80636544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5318,7 +5251,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5554,24 +5487,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="70207360"/>
-        <c:axId val="70208896"/>
+        <c:axId val="80679680"/>
+        <c:axId val="80681216"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="70207360"/>
+        <c:axId val="80679680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70208896"/>
+        <c:crossAx val="80681216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70208896"/>
+        <c:axId val="80681216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5579,20 +5512,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70207360"/>
+        <c:crossAx val="80679680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6119,7 +6051,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -6398,8 +6330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6407,7 +6339,7 @@
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
@@ -6481,7 +6413,7 @@
       <c r="H4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="119" t="s">
+      <c r="I4" s="118" t="s">
         <v>24</v>
       </c>
       <c r="J4" s="17" t="s">
@@ -6508,7 +6440,7 @@
       <c r="E5" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="72" t="s">
         <v>72</v>
       </c>
       <c r="G5" s="9"/>
@@ -6535,7 +6467,7 @@
       <c r="I6" s="124"/>
       <c r="J6" s="124"/>
     </row>
-    <row r="7" spans="1:13" ht="92.25">
+    <row r="7" spans="1:13" ht="46.5">
       <c r="A7" s="23" t="s">
         <v>14</v>
       </c>
@@ -6545,8 +6477,8 @@
       <c r="C7" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="29">
-        <v>72</v>
+      <c r="D7" s="139" t="s">
+        <v>193</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
@@ -6574,25 +6506,25 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="34.5">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="120" t="s">
+      <c r="E10" s="119" t="s">
         <v>188</v>
       </c>
-      <c r="F10" s="121" t="s">
+      <c r="F10" s="120" t="s">
         <v>189</v>
       </c>
-      <c r="G10" s="122" t="s">
+      <c r="G10" s="121" t="s">
         <v>190</v>
       </c>
     </row>
@@ -6602,13 +6534,13 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="31" t="s">
         <v>29</v>
       </c>
     </row>
@@ -6618,88 +6550,88 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="127.5">
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="42" t="s">
         <v>45</v>
       </c>
       <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:13" ht="128.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="43" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="128.25">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="44" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18.75">
-      <c r="A19" s="38"/>
-      <c r="B19" s="38"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
     </row>
     <row r="20" spans="1:4" ht="21">
       <c r="A20" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D20" s="92"/>
+      <c r="D20" s="91"/>
     </row>
     <row r="21" spans="1:4" ht="18.75">
-      <c r="A21" s="38"/>
-      <c r="B21" s="92" t="s">
+      <c r="A21" s="37"/>
+      <c r="B21" s="91" t="s">
         <v>152</v>
       </c>
-      <c r="C21" s="92"/>
-      <c r="D21" s="92"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
     </row>
     <row r="22" spans="1:4" ht="20.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="92" t="s">
+      <c r="A22" s="37"/>
+      <c r="B22" s="91" t="s">
         <v>152</v>
       </c>
-      <c r="C22" s="93" t="s">
+      <c r="C22" s="92" t="s">
         <v>154</v>
       </c>
-      <c r="D22" s="92"/>
+      <c r="D22" s="91"/>
     </row>
     <row r="23" spans="1:4" ht="18.75">
-      <c r="A23" s="38"/>
-      <c r="B23" s="92"/>
-      <c r="C23" s="92"/>
-      <c r="D23" s="92"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
     </row>
     <row r="24" spans="1:4" ht="21">
       <c r="A24" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B24" s="92"/>
-      <c r="C24" s="92"/>
-      <c r="D24" s="92"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="91"/>
     </row>
     <row r="25" spans="1:4" ht="76.5">
       <c r="A25" s="4"/>
-      <c r="B25" s="94" t="s">
+      <c r="B25" s="93" t="s">
         <v>155</v>
       </c>
-      <c r="C25" s="92"/>
-      <c r="D25" s="92"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
     </row>
     <row r="26" spans="1:4" ht="60">
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="93" t="s">
         <v>182</v>
       </c>
     </row>
@@ -6707,13 +6639,13 @@
       <c r="A27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="48" t="s">
+      <c r="D27" s="47" t="s">
         <v>56</v>
       </c>
     </row>
@@ -6721,13 +6653,13 @@
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="50" t="s">
+      <c r="C28" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="51" t="s">
+      <c r="D28" s="50" t="s">
         <v>51</v>
       </c>
     </row>
@@ -6735,13 +6667,13 @@
       <c r="A29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="52" t="s">
+      <c r="B29" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C29" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="51" t="s">
+      <c r="D29" s="50" t="s">
         <v>55</v>
       </c>
     </row>
@@ -6749,7 +6681,7 @@
       <c r="A31" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="57" t="s">
         <v>63</v>
       </c>
     </row>
@@ -6780,7 +6712,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1" ht="18.75">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="87" t="s">
         <v>139</v>
       </c>
     </row>
@@ -6790,7 +6722,7 @@
       </c>
     </row>
     <row r="20" spans="1:1" ht="18.75">
-      <c r="A20" s="88" t="s">
+      <c r="A20" s="87" t="s">
         <v>140</v>
       </c>
     </row>
@@ -6825,10 +6757,10 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="33"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3" hidden="1">
       <c r="B2" t="s">
@@ -6917,7 +6849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -6937,7 +6869,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="122" t="s">
         <v>69</v>
       </c>
     </row>
@@ -6975,211 +6907,211 @@
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="56" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21">
       <c r="A2" s="4"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
     </row>
     <row r="3" spans="1:7" ht="21">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="62" t="s">
+      <c r="E3" s="61" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="B5" s="99" t="s">
+      <c r="B5" s="98" t="s">
         <v>191</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="99" t="s">
         <v>192</v>
       </c>
-      <c r="D5" s="103" t="s">
+      <c r="D5" s="102" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="64" t="s">
+      <c r="E9" s="63" t="s">
         <v>165</v>
       </c>
-      <c r="F9" s="65" t="s">
+      <c r="F9" s="64" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="67"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="66"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="66" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="G12" s="59"/>
+      <c r="C12" s="65"/>
+      <c r="G12" s="58"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="B13" s="65"/>
-      <c r="C13" s="64"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="63"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="B15" s="113" t="s">
+      <c r="B15" s="112" t="s">
         <v>176</v>
       </c>
-      <c r="C15" s="114"/>
+      <c r="C15" s="113"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="B16" s="115" t="s">
+      <c r="B16" s="114" t="s">
         <v>177</v>
       </c>
-      <c r="C16" s="116"/>
+      <c r="C16" s="115"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
     </row>
     <row r="19" spans="1:8" ht="15.75">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="D19" s="65" t="s">
+      <c r="D19" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="67" t="s">
+      <c r="F19" s="66" t="s">
         <v>158</v>
       </c>
-      <c r="G19" s="95" t="s">
+      <c r="G19" s="94" t="s">
         <v>159</v>
       </c>
-      <c r="H19" s="66" t="s">
+      <c r="H19" s="65" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" s="61"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="62"/>
-      <c r="F20" s="96"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="97"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="61"/>
+      <c r="F20" s="95"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="96"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="66"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="67"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="64"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="66"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="63"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="B23" s="108" t="s">
+      <c r="B23" s="107" t="s">
         <v>161</v>
       </c>
-      <c r="C23" s="108" t="s">
+      <c r="C23" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="108" t="s">
+      <c r="D23" s="107" t="s">
         <v>158</v>
       </c>
-      <c r="F23" s="109" t="s">
+      <c r="F23" s="108" t="s">
         <v>162</v>
       </c>
-      <c r="G23" s="109" t="s">
+      <c r="G23" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="H23" s="109" t="s">
+      <c r="H23" s="108" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="B24" s="108" t="s">
+      <c r="B24" s="107" t="s">
         <v>161</v>
       </c>
-      <c r="C24" s="108" t="s">
+      <c r="C24" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="108" t="s">
+      <c r="D24" s="107" t="s">
         <v>158</v>
       </c>
-      <c r="F24" s="109" t="s">
+      <c r="F24" s="108" t="s">
         <v>162</v>
       </c>
-      <c r="G24" s="109" t="s">
+      <c r="G24" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="H24" s="109" t="s">
+      <c r="H24" s="108" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="B25" s="108" t="s">
+      <c r="B25" s="107" t="s">
         <v>161</v>
       </c>
-      <c r="C25" s="108" t="s">
+      <c r="C25" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="108" t="s">
+      <c r="D25" s="107" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="109" t="s">
+      <c r="F25" s="108" t="s">
         <v>162</v>
       </c>
-      <c r="G25" s="109" t="s">
+      <c r="G25" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="H25" s="109" t="s">
+      <c r="H25" s="108" t="s">
         <v>158</v>
       </c>
     </row>
@@ -7251,9 +7183,9 @@
   <sheetData>
     <row r="2" spans="1:9" ht="21">
       <c r="A2" s="4"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
     </row>
     <row r="3" spans="1:9" ht="21">
       <c r="A3" s="4" t="s">
@@ -7261,100 +7193,100 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="101" t="s">
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="E4" s="102" t="s">
+      <c r="E4" s="101" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1">
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="116" t="s">
         <v>170</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="117" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="104" t="s">
+      <c r="D5" s="103" t="s">
         <v>168</v>
       </c>
-      <c r="E5" s="105" t="s">
+      <c r="E5" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="106" t="s">
+      <c r="F5" s="105" t="s">
         <v>187</v>
       </c>
-      <c r="G5" s="107" t="s">
+      <c r="G5" s="106" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="72" t="s">
+      <c r="E8" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="72" t="s">
+      <c r="F8" s="71" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B9" s="70"/>
-      <c r="C9" s="71"/>
-      <c r="E9" s="72" t="s">
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
+      <c r="E9" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="71" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="G11" s="59"/>
+      <c r="G11" s="58"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="111" t="s">
         <v>174</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="E12" s="110" t="s">
+      <c r="E12" s="109" t="s">
         <v>163</v>
       </c>
-      <c r="F12" s="110" t="s">
+      <c r="F12" s="109" t="s">
         <v>164</v>
       </c>
-      <c r="H12" s="111" t="s">
+      <c r="H12" s="110" t="s">
         <v>163</v>
       </c>
-      <c r="I12" s="111" t="s">
+      <c r="I12" s="110" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="E13" s="110" t="s">
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="E13" s="109" t="s">
         <v>172</v>
       </c>
-      <c r="F13" s="110"/>
-      <c r="H13" s="111" t="s">
+      <c r="F13" s="109"/>
+      <c r="H13" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="I13" s="111"/>
+      <c r="I13" s="110"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7367,7 +7299,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7385,70 +7317,70 @@
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="85" t="s">
+      <c r="D1" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="85" t="s">
+      <c r="E1" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="85" t="s">
+      <c r="F1" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="85" t="s">
+      <c r="G1" s="84" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="B2" s="75">
+      <c r="B2" s="74">
         <v>1234.56</v>
       </c>
-      <c r="C2" s="76">
+      <c r="C2" s="75">
         <v>1234.56</v>
       </c>
-      <c r="D2" s="77">
+      <c r="D2" s="76">
         <v>1234</v>
       </c>
-      <c r="E2" s="74">
+      <c r="E2" s="73">
         <v>41376</v>
       </c>
-      <c r="F2" s="78">
+      <c r="F2" s="77">
         <v>0.7583333333333333</v>
       </c>
-      <c r="G2" s="79">
+      <c r="G2" s="78">
         <v>0.123</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="85" t="s">
+      <c r="D3" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="84" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="B4" s="80">
+      <c r="B4" s="79">
         <v>0.48</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="80">
         <v>1000000000</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="83">
+      <c r="E4" s="82">
         <v>73504450</v>
       </c>
     </row>
@@ -7458,7 +7390,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="85" t="s">
+      <c r="A7" s="84" t="s">
         <v>91</v>
       </c>
       <c r="B7">
@@ -7466,7 +7398,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="84" t="s">
         <v>166</v>
       </c>
       <c r="B8" t="s">
@@ -7489,15 +7421,15 @@
       <c r="A11" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="84" t="s">
         <v>179</v>
       </c>
       <c r="C11">
         <f>SUM(TestRange1)</f>
         <v>21</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="F11" s="85" t="s">
+      <c r="D11" s="58"/>
+      <c r="F11" s="84" t="s">
         <v>180</v>
       </c>
       <c r="G11">
@@ -7506,13 +7438,13 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="B12" s="64">
+      <c r="B12" s="63">
         <v>1</v>
       </c>
-      <c r="C12" s="60">
+      <c r="C12" s="59">
         <v>2</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D12" s="64">
         <v>3</v>
       </c>
       <c r="F12" s="131">
@@ -7522,13 +7454,13 @@
       <c r="H12" s="132"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="B13" s="66">
+      <c r="B13" s="65">
         <v>4</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="53">
         <v>5</v>
       </c>
-      <c r="D13" s="67">
+      <c r="D13" s="66">
         <v>6</v>
       </c>
       <c r="F13" s="135"/>
@@ -7550,9 +7482,9 @@
   <mergeCells count="1">
     <mergeCell ref="F12:H13"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="not a valid grade" error="not a valid grade" promptTitle="4 grades only" prompt="input a grade score" sqref="B8">
-      <formula1>$C$88:$F$88</formula1>
+      <formula1>$C$8:$F$8</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sorry" error="1 - 10" prompt="valid between 1 to 10" sqref="B7">
       <formula1>1</formula1>
@@ -7580,10 +7512,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="42">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="86" t="s">
         <v>97</v>
       </c>
       <c r="C1" t="str">
@@ -7592,8 +7524,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="31.5">
-      <c r="A2" s="86"/>
-      <c r="B2" s="87" t="s">
+      <c r="A2" s="85"/>
+      <c r="B2" s="86" t="s">
         <v>183</v>
       </c>
       <c r="C2">
@@ -7602,14 +7534,14 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="21">
-      <c r="A3" s="86"/>
-      <c r="B3" s="87"/>
+      <c r="A3" s="85"/>
+      <c r="B3" s="86"/>
     </row>
     <row r="4" spans="1:3" ht="61.5">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="85" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="86" t="s">
         <v>184</v>
       </c>
       <c r="C4" t="str">
@@ -7618,7 +7550,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="45">
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="86" t="s">
         <v>185</v>
       </c>
       <c r="C5">
@@ -7784,10 +7716,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="61.5" customHeight="1">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="83" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="83" t="s">
         <v>146</v>
       </c>
       <c r="C3" t="s">
@@ -7854,7 +7786,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="87" t="s">
         <v>106</v>
       </c>
       <c r="N12" t="s">
@@ -7862,16 +7794,16 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A13" s="90" t="s">
+      <c r="A13" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="91" t="s">
+      <c r="B13" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="91" t="s">
+      <c r="C13" s="90" t="s">
         <v>98</v>
       </c>
-      <c r="D13" s="91" t="s">
+      <c r="D13" s="90" t="s">
         <v>99</v>
       </c>
     </row>
@@ -7879,13 +7811,13 @@
       <c r="A14" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="89">
+      <c r="B14" s="88">
         <v>0.3427</v>
       </c>
-      <c r="C14" s="89">
+      <c r="C14" s="88">
         <v>0.25990000000000002</v>
       </c>
-      <c r="D14" s="89">
+      <c r="D14" s="88">
         <v>0.2268</v>
       </c>
     </row>
@@ -7893,13 +7825,13 @@
       <c r="A15" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="89">
+      <c r="B15" s="88">
         <v>0.32700000000000001</v>
       </c>
-      <c r="C15" s="89">
+      <c r="C15" s="88">
         <v>0.27239999999999998</v>
       </c>
-      <c r="D15" s="89">
+      <c r="D15" s="88">
         <v>0.2276</v>
       </c>
     </row>
@@ -7907,13 +7839,13 @@
       <c r="A16" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="89">
+      <c r="B16" s="88">
         <v>0.31680000000000003</v>
       </c>
-      <c r="C16" s="89">
+      <c r="C16" s="88">
         <v>0.28089999999999998</v>
       </c>
-      <c r="D16" s="89">
+      <c r="D16" s="88">
         <v>0.2273</v>
       </c>
     </row>
@@ -7921,13 +7853,13 @@
       <c r="A17" t="s">
         <v>128</v>
       </c>
-      <c r="B17" s="89">
+      <c r="B17" s="88">
         <v>0.30809999999999998</v>
       </c>
-      <c r="C17" s="89">
+      <c r="C17" s="88">
         <v>0.28239999999999998</v>
       </c>
-      <c r="D17" s="89">
+      <c r="D17" s="88">
         <v>0.22489999999999999</v>
       </c>
     </row>
@@ -7935,13 +7867,13 @@
       <c r="A18" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="89">
+      <c r="B18" s="88">
         <v>0.28870000000000001</v>
       </c>
-      <c r="C18" s="89">
+      <c r="C18" s="88">
         <v>0.29149999999999998</v>
       </c>
-      <c r="D18" s="89">
+      <c r="D18" s="88">
         <v>0.22969999999999999</v>
       </c>
     </row>
@@ -7949,13 +7881,13 @@
       <c r="A19" t="s">
         <v>126</v>
       </c>
-      <c r="B19" s="89">
+      <c r="B19" s="88">
         <v>0.28949999999999998</v>
       </c>
-      <c r="C19" s="89">
+      <c r="C19" s="88">
         <v>0.29349999999999998</v>
       </c>
-      <c r="D19" s="89">
+      <c r="D19" s="88">
         <v>0.22</v>
       </c>
     </row>
@@ -7963,13 +7895,13 @@
       <c r="A20" t="s">
         <v>125</v>
       </c>
-      <c r="B20" s="89">
+      <c r="B20" s="88">
         <v>0.28489999999999999</v>
       </c>
-      <c r="C20" s="89">
+      <c r="C20" s="88">
         <v>0.30059999999999998</v>
       </c>
-      <c r="D20" s="89">
+      <c r="D20" s="88">
         <v>0.21010000000000001</v>
       </c>
     </row>
@@ -7977,13 +7909,13 @@
       <c r="A21" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="89">
+      <c r="B21" s="88">
         <v>0.2898</v>
       </c>
-      <c r="C21" s="89">
+      <c r="C21" s="88">
         <v>0.29630000000000001</v>
       </c>
-      <c r="D21" s="89">
+      <c r="D21" s="88">
         <v>0.2016</v>
       </c>
     </row>
@@ -7991,13 +7923,13 @@
       <c r="A22" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="89">
+      <c r="B22" s="88">
         <v>0.28770000000000001</v>
       </c>
-      <c r="C22" s="89">
+      <c r="C22" s="88">
         <v>0.30009999999999998</v>
       </c>
-      <c r="D22" s="89">
+      <c r="D22" s="88">
         <v>0.19700000000000001</v>
       </c>
     </row>
@@ -8005,13 +7937,13 @@
       <c r="A23" t="s">
         <v>122</v>
       </c>
-      <c r="B23" s="89">
+      <c r="B23" s="88">
         <v>0.28129999999999999</v>
       </c>
-      <c r="C23" s="89">
+      <c r="C23" s="88">
         <v>0.3049</v>
       </c>
-      <c r="D23" s="89">
+      <c r="D23" s="88">
         <v>0.19570000000000001</v>
       </c>
     </row>
@@ -8019,13 +7951,13 @@
       <c r="A24" t="s">
         <v>121</v>
       </c>
-      <c r="B24" s="89">
+      <c r="B24" s="88">
         <v>0.27150000000000002</v>
       </c>
-      <c r="C24" s="89">
+      <c r="C24" s="88">
         <v>0.3105</v>
       </c>
-      <c r="D24" s="89">
+      <c r="D24" s="88">
         <v>0.19739999999999999</v>
       </c>
     </row>
@@ -8033,13 +7965,13 @@
       <c r="A25" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="89">
+      <c r="B25" s="88">
         <v>0.26300000000000001</v>
       </c>
-      <c r="C25" s="89">
+      <c r="C25" s="88">
         <v>0.31119999999999998</v>
       </c>
-      <c r="D25" s="89">
+      <c r="D25" s="88">
         <v>0.18709999999999999</v>
       </c>
     </row>
@@ -8047,13 +7979,13 @@
       <c r="A26" t="s">
         <v>119</v>
       </c>
-      <c r="B26" s="89">
+      <c r="B26" s="88">
         <v>0.26369999999999999</v>
       </c>
-      <c r="C26" s="89">
+      <c r="C26" s="88">
         <v>0.31509999999999999</v>
       </c>
-      <c r="D26" s="89">
+      <c r="D26" s="88">
         <v>0.18390000000000001</v>
       </c>
     </row>
@@ -8061,13 +7993,13 @@
       <c r="A27" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="89">
+      <c r="B27" s="88">
         <v>0.25540000000000002</v>
       </c>
-      <c r="C27" s="89">
+      <c r="C27" s="88">
         <v>0.3196</v>
       </c>
-      <c r="D27" s="89">
+      <c r="D27" s="88">
         <v>0.18279999999999999</v>
       </c>
     </row>
@@ -8075,18 +8007,18 @@
       <c r="A28" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="89">
+      <c r="B28" s="88">
         <v>0.25080000000000002</v>
       </c>
-      <c r="C28" s="89">
+      <c r="C28" s="88">
         <v>0.32879999999999998</v>
       </c>
-      <c r="D28" s="89">
+      <c r="D28" s="88">
         <v>0.17860000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="18.75">
-      <c r="A32" s="88" t="s">
+      <c r="A32" s="87" t="s">
         <v>113</v>
       </c>
       <c r="D32" t="s">
@@ -8097,7 +8029,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="85" t="s">
+      <c r="A33" s="84" t="s">
         <v>101</v>
       </c>
     </row>
@@ -8150,7 +8082,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="18.75">
-      <c r="A48" s="88" t="s">
+      <c r="A48" s="87" t="s">
         <v>107</v>
       </c>
     </row>
@@ -8160,7 +8092,7 @@
       </c>
     </row>
     <row r="69" spans="1:12" ht="18.75">
-      <c r="A69" s="88" t="s">
+      <c r="A69" s="87" t="s">
         <v>108</v>
       </c>
     </row>
@@ -8175,12 +8107,12 @@
       </c>
     </row>
     <row r="95" spans="1:12" ht="18.75">
-      <c r="A95" s="88" t="s">
+      <c r="A95" s="87" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="18.75">
-      <c r="A117" s="88" t="s">
+      <c r="A117" s="87" t="s">
         <v>110</v>
       </c>
     </row>
@@ -8190,7 +8122,7 @@
       </c>
     </row>
     <row r="137" spans="1:1" ht="18.75">
-      <c r="A137" s="88" t="s">
+      <c r="A137" s="87" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>